<commit_message>
First full working implementation
</commit_message>
<xml_diff>
--- a/CPC_core_data.xlsx
+++ b/CPC_core_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Processes\TCAC\TCAC13 simulations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\dev\git\BitBucket workspaces\IOTC-ws\IOTC working parties\iotc-tcac-simulations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD2BBD9A-3E81-423A-ABB0-3E8D800A299B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C24E6931-CEA9-47E2-887F-11C72853DD1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{37AF7B81-AA52-434F-A73C-A9320683B607}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="98">
   <si>
     <t>SIDS</t>
   </si>
@@ -250,15 +250,6 @@
   </si>
   <si>
     <t>CUV_INDEX</t>
-  </si>
-  <si>
-    <t>PROPORTION_WORKERS_EMPLOYED_SSF</t>
-  </si>
-  <si>
-    <t>FISHERIES_CONTRIBUTION_GDP</t>
-  </si>
-  <si>
-    <t>PROPORTION_EXPORT_VALUE_FISHERY</t>
   </si>
   <si>
     <t>HDI_STATUS</t>
@@ -371,6 +362,18 @@
   <si>
     <t>https://datahelpdesk.worldbank.org/knowledgebase/articles/906519-world-bank-country-and-lending-group</t>
   </si>
+  <si>
+    <t>PROP_WORKERS_EMPLOYED_SSF</t>
+  </si>
+  <si>
+    <t>PROP_FISHERIES_CONTRIBUTION_GDP</t>
+  </si>
+  <si>
+    <t>PROP_EXPORT_VALUE_FISHERY</t>
+  </si>
+  <si>
+    <t>Dummy values, waiting for actual values to be provided by the proponents</t>
+  </si>
 </sst>
 </file>
 
@@ -379,7 +382,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -416,6 +419,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -439,7 +449,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -452,13 +462,16 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -806,7 +819,7 @@
         <v>66</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>0</v>
@@ -815,24 +828,24 @@
         <v>67</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="J1" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="8"/>
-      <c r="R1" s="8"/>
-      <c r="S1" s="8"/>
-      <c r="T1" s="8"/>
-      <c r="U1" s="8"/>
-      <c r="V1" s="8"/>
-      <c r="W1" s="8"/>
+        <v>85</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="9"/>
+      <c r="S1" s="9"/>
+      <c r="T1" s="9"/>
+      <c r="U1" s="9"/>
+      <c r="V1" s="9"/>
+      <c r="W1" s="9"/>
     </row>
     <row r="2" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -859,21 +872,21 @@
       <c r="H2" s="2">
         <v>7.6899999999999996E-2</v>
       </c>
-      <c r="J2" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="9"/>
-      <c r="O2" s="9"/>
-      <c r="P2" s="9"/>
-      <c r="Q2" s="9"/>
-      <c r="R2" s="9"/>
-      <c r="S2" s="9"/>
-      <c r="T2" s="9"/>
-      <c r="U2" s="9"/>
-      <c r="V2" s="9"/>
+      <c r="J2" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="10"/>
+      <c r="P2" s="10"/>
+      <c r="Q2" s="10"/>
+      <c r="R2" s="10"/>
+      <c r="S2" s="10"/>
+      <c r="T2" s="10"/>
+      <c r="U2" s="10"/>
+      <c r="V2" s="10"/>
       <c r="W2" s="5"/>
       <c r="X2" s="5"/>
       <c r="Y2" s="5"/>
@@ -904,19 +917,19 @@
       <c r="H3" s="2">
         <v>1.2999999999999999E-3</v>
       </c>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="9"/>
-      <c r="N3" s="9"/>
-      <c r="O3" s="9"/>
-      <c r="P3" s="9"/>
-      <c r="Q3" s="9"/>
-      <c r="R3" s="9"/>
-      <c r="S3" s="9"/>
-      <c r="T3" s="9"/>
-      <c r="U3" s="9"/>
-      <c r="V3" s="9"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="10"/>
+      <c r="R3" s="10"/>
+      <c r="S3" s="10"/>
+      <c r="T3" s="10"/>
+      <c r="U3" s="10"/>
+      <c r="V3" s="10"/>
       <c r="W3" s="5"/>
       <c r="X3" s="5"/>
       <c r="Y3" s="5"/>
@@ -947,19 +960,19 @@
       <c r="H4" s="2">
         <v>0</v>
       </c>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="9"/>
-      <c r="N4" s="9"/>
-      <c r="O4" s="9"/>
-      <c r="P4" s="9"/>
-      <c r="Q4" s="9"/>
-      <c r="R4" s="9"/>
-      <c r="S4" s="9"/>
-      <c r="T4" s="9"/>
-      <c r="U4" s="9"/>
-      <c r="V4" s="9"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="10"/>
+      <c r="S4" s="10"/>
+      <c r="T4" s="10"/>
+      <c r="U4" s="10"/>
+      <c r="V4" s="10"/>
       <c r="W4" s="5"/>
       <c r="X4" s="5"/>
       <c r="Y4" s="5"/>
@@ -990,19 +1003,19 @@
       <c r="H5" s="2">
         <v>2.7000000000000001E-3</v>
       </c>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="9"/>
-      <c r="M5" s="9"/>
-      <c r="N5" s="9"/>
-      <c r="O5" s="9"/>
-      <c r="P5" s="9"/>
-      <c r="Q5" s="9"/>
-      <c r="R5" s="9"/>
-      <c r="S5" s="9"/>
-      <c r="T5" s="9"/>
-      <c r="U5" s="9"/>
-      <c r="V5" s="9"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="10"/>
+      <c r="P5" s="10"/>
+      <c r="Q5" s="10"/>
+      <c r="R5" s="10"/>
+      <c r="S5" s="10"/>
+      <c r="T5" s="10"/>
+      <c r="U5" s="10"/>
+      <c r="V5" s="10"/>
       <c r="W5" s="5"/>
       <c r="X5" s="5"/>
       <c r="Y5" s="5"/>
@@ -1033,19 +1046,19 @@
       <c r="H6" s="2">
         <v>6.1000000000000004E-3</v>
       </c>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="9"/>
-      <c r="M6" s="9"/>
-      <c r="N6" s="9"/>
-      <c r="O6" s="9"/>
-      <c r="P6" s="9"/>
-      <c r="Q6" s="9"/>
-      <c r="R6" s="9"/>
-      <c r="S6" s="9"/>
-      <c r="T6" s="9"/>
-      <c r="U6" s="9"/>
-      <c r="V6" s="9"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="10"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="10"/>
+      <c r="R6" s="10"/>
+      <c r="S6" s="10"/>
+      <c r="T6" s="10"/>
+      <c r="U6" s="10"/>
+      <c r="V6" s="10"/>
       <c r="W6" s="5"/>
       <c r="X6" s="5"/>
       <c r="Y6" s="5"/>
@@ -1076,19 +1089,19 @@
       <c r="H7" s="2">
         <v>3.6900000000000002E-2</v>
       </c>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9"/>
-      <c r="L7" s="9"/>
-      <c r="M7" s="9"/>
-      <c r="N7" s="9"/>
-      <c r="O7" s="9"/>
-      <c r="P7" s="9"/>
-      <c r="Q7" s="9"/>
-      <c r="R7" s="9"/>
-      <c r="S7" s="9"/>
-      <c r="T7" s="9"/>
-      <c r="U7" s="9"/>
-      <c r="V7" s="9"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="10"/>
+      <c r="S7" s="10"/>
+      <c r="T7" s="10"/>
+      <c r="U7" s="10"/>
+      <c r="V7" s="10"/>
       <c r="W7" s="5"/>
       <c r="X7" s="5"/>
       <c r="Y7" s="5"/>
@@ -1119,19 +1132,19 @@
       <c r="H8" s="2">
         <v>1.04E-2</v>
       </c>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="9"/>
-      <c r="M8" s="9"/>
-      <c r="N8" s="9"/>
-      <c r="O8" s="9"/>
-      <c r="P8" s="9"/>
-      <c r="Q8" s="9"/>
-      <c r="R8" s="9"/>
-      <c r="S8" s="9"/>
-      <c r="T8" s="9"/>
-      <c r="U8" s="9"/>
-      <c r="V8" s="9"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="10"/>
+      <c r="S8" s="10"/>
+      <c r="T8" s="10"/>
+      <c r="U8" s="10"/>
+      <c r="V8" s="10"/>
       <c r="W8" s="5"/>
       <c r="X8" s="5"/>
       <c r="Y8" s="5"/>
@@ -1162,19 +1175,19 @@
       <c r="H9" s="2">
         <v>3.1600000000000003E-2</v>
       </c>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="9"/>
-      <c r="M9" s="9"/>
-      <c r="N9" s="9"/>
-      <c r="O9" s="9"/>
-      <c r="P9" s="9"/>
-      <c r="Q9" s="9"/>
-      <c r="R9" s="9"/>
-      <c r="S9" s="9"/>
-      <c r="T9" s="9"/>
-      <c r="U9" s="9"/>
-      <c r="V9" s="9"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="10"/>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="10"/>
+      <c r="R9" s="10"/>
+      <c r="S9" s="10"/>
+      <c r="T9" s="10"/>
+      <c r="U9" s="10"/>
+      <c r="V9" s="10"/>
       <c r="W9" s="5"/>
       <c r="X9" s="5"/>
       <c r="Y9" s="5"/>
@@ -1205,19 +1218,19 @@
       <c r="H10" s="2">
         <v>3.7100000000000001E-2</v>
       </c>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
-      <c r="M10" s="9"/>
-      <c r="N10" s="9"/>
-      <c r="O10" s="9"/>
-      <c r="P10" s="9"/>
-      <c r="Q10" s="9"/>
-      <c r="R10" s="9"/>
-      <c r="S10" s="9"/>
-      <c r="T10" s="9"/>
-      <c r="U10" s="9"/>
-      <c r="V10" s="9"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="10"/>
+      <c r="O10" s="10"/>
+      <c r="P10" s="10"/>
+      <c r="Q10" s="10"/>
+      <c r="R10" s="10"/>
+      <c r="S10" s="10"/>
+      <c r="T10" s="10"/>
+      <c r="U10" s="10"/>
+      <c r="V10" s="10"/>
       <c r="W10" s="5"/>
       <c r="X10" s="5"/>
       <c r="Y10" s="5"/>
@@ -1248,19 +1261,19 @@
       <c r="H11" s="2">
         <v>2.5999999999999999E-3</v>
       </c>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="9"/>
-      <c r="M11" s="9"/>
-      <c r="N11" s="9"/>
-      <c r="O11" s="9"/>
-      <c r="P11" s="9"/>
-      <c r="Q11" s="9"/>
-      <c r="R11" s="9"/>
-      <c r="S11" s="9"/>
-      <c r="T11" s="9"/>
-      <c r="U11" s="9"/>
-      <c r="V11" s="9"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="10"/>
+      <c r="Q11" s="10"/>
+      <c r="R11" s="10"/>
+      <c r="S11" s="10"/>
+      <c r="T11" s="10"/>
+      <c r="U11" s="10"/>
+      <c r="V11" s="10"/>
       <c r="W11" s="5"/>
       <c r="X11" s="5"/>
       <c r="Y11" s="5"/>
@@ -1291,19 +1304,19 @@
       <c r="H12" s="2">
         <v>0</v>
       </c>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="9"/>
-      <c r="M12" s="9"/>
-      <c r="N12" s="9"/>
-      <c r="O12" s="9"/>
-      <c r="P12" s="9"/>
-      <c r="Q12" s="9"/>
-      <c r="R12" s="9"/>
-      <c r="S12" s="9"/>
-      <c r="T12" s="9"/>
-      <c r="U12" s="9"/>
-      <c r="V12" s="9"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
+      <c r="N12" s="10"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="10"/>
+      <c r="Q12" s="10"/>
+      <c r="R12" s="10"/>
+      <c r="S12" s="10"/>
+      <c r="T12" s="10"/>
+      <c r="U12" s="10"/>
+      <c r="V12" s="10"/>
       <c r="W12" s="5"/>
       <c r="X12" s="5"/>
       <c r="Y12" s="5"/>
@@ -1334,19 +1347,19 @@
       <c r="H13" s="2">
         <v>1.8E-3</v>
       </c>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="9"/>
-      <c r="M13" s="9"/>
-      <c r="N13" s="9"/>
-      <c r="O13" s="9"/>
-      <c r="P13" s="9"/>
-      <c r="Q13" s="9"/>
-      <c r="R13" s="9"/>
-      <c r="S13" s="9"/>
-      <c r="T13" s="9"/>
-      <c r="U13" s="9"/>
-      <c r="V13" s="9"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="10"/>
+      <c r="P13" s="10"/>
+      <c r="Q13" s="10"/>
+      <c r="R13" s="10"/>
+      <c r="S13" s="10"/>
+      <c r="T13" s="10"/>
+      <c r="U13" s="10"/>
+      <c r="V13" s="10"/>
       <c r="W13" s="5"/>
       <c r="X13" s="5"/>
       <c r="Y13" s="5"/>
@@ -1377,19 +1390,19 @@
       <c r="H14" s="2">
         <v>0</v>
       </c>
-      <c r="J14" s="9"/>
-      <c r="K14" s="9"/>
-      <c r="L14" s="9"/>
-      <c r="M14" s="9"/>
-      <c r="N14" s="9"/>
-      <c r="O14" s="9"/>
-      <c r="P14" s="9"/>
-      <c r="Q14" s="9"/>
-      <c r="R14" s="9"/>
-      <c r="S14" s="9"/>
-      <c r="T14" s="9"/>
-      <c r="U14" s="9"/>
-      <c r="V14" s="9"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+      <c r="N14" s="10"/>
+      <c r="O14" s="10"/>
+      <c r="P14" s="10"/>
+      <c r="Q14" s="10"/>
+      <c r="R14" s="10"/>
+      <c r="S14" s="10"/>
+      <c r="T14" s="10"/>
+      <c r="U14" s="10"/>
+      <c r="V14" s="10"/>
       <c r="W14" s="5"/>
       <c r="X14" s="5"/>
       <c r="Y14" s="5"/>
@@ -1420,19 +1433,19 @@
       <c r="H15" s="2">
         <v>0</v>
       </c>
-      <c r="J15" s="9"/>
-      <c r="K15" s="9"/>
-      <c r="L15" s="9"/>
-      <c r="M15" s="9"/>
-      <c r="N15" s="9"/>
-      <c r="O15" s="9"/>
-      <c r="P15" s="9"/>
-      <c r="Q15" s="9"/>
-      <c r="R15" s="9"/>
-      <c r="S15" s="9"/>
-      <c r="T15" s="9"/>
-      <c r="U15" s="9"/>
-      <c r="V15" s="9"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="10"/>
+      <c r="O15" s="10"/>
+      <c r="P15" s="10"/>
+      <c r="Q15" s="10"/>
+      <c r="R15" s="10"/>
+      <c r="S15" s="10"/>
+      <c r="T15" s="10"/>
+      <c r="U15" s="10"/>
+      <c r="V15" s="10"/>
       <c r="W15" s="5"/>
       <c r="X15" s="5"/>
       <c r="Y15" s="5"/>
@@ -1463,19 +1476,19 @@
       <c r="H16" s="2">
         <v>8.6E-3</v>
       </c>
-      <c r="J16" s="9"/>
-      <c r="K16" s="9"/>
-      <c r="L16" s="9"/>
-      <c r="M16" s="9"/>
-      <c r="N16" s="9"/>
-      <c r="O16" s="9"/>
-      <c r="P16" s="9"/>
-      <c r="Q16" s="9"/>
-      <c r="R16" s="9"/>
-      <c r="S16" s="9"/>
-      <c r="T16" s="9"/>
-      <c r="U16" s="9"/>
-      <c r="V16" s="9"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="10"/>
+      <c r="N16" s="10"/>
+      <c r="O16" s="10"/>
+      <c r="P16" s="10"/>
+      <c r="Q16" s="10"/>
+      <c r="R16" s="10"/>
+      <c r="S16" s="10"/>
+      <c r="T16" s="10"/>
+      <c r="U16" s="10"/>
+      <c r="V16" s="10"/>
       <c r="W16" s="5"/>
       <c r="X16" s="5"/>
       <c r="Y16" s="5"/>
@@ -1506,19 +1519,19 @@
       <c r="H17" s="2">
         <v>1.95E-2</v>
       </c>
-      <c r="J17" s="9"/>
-      <c r="K17" s="9"/>
-      <c r="L17" s="9"/>
-      <c r="M17" s="9"/>
-      <c r="N17" s="9"/>
-      <c r="O17" s="9"/>
-      <c r="P17" s="9"/>
-      <c r="Q17" s="9"/>
-      <c r="R17" s="9"/>
-      <c r="S17" s="9"/>
-      <c r="T17" s="9"/>
-      <c r="U17" s="9"/>
-      <c r="V17" s="9"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="10"/>
+      <c r="N17" s="10"/>
+      <c r="O17" s="10"/>
+      <c r="P17" s="10"/>
+      <c r="Q17" s="10"/>
+      <c r="R17" s="10"/>
+      <c r="S17" s="10"/>
+      <c r="T17" s="10"/>
+      <c r="U17" s="10"/>
+      <c r="V17" s="10"/>
       <c r="W17" s="5"/>
       <c r="X17" s="5"/>
       <c r="Y17" s="5"/>
@@ -1549,19 +1562,19 @@
       <c r="H18" s="2">
         <v>1.49E-2</v>
       </c>
-      <c r="J18" s="9"/>
-      <c r="K18" s="9"/>
-      <c r="L18" s="9"/>
-      <c r="M18" s="9"/>
-      <c r="N18" s="9"/>
-      <c r="O18" s="9"/>
-      <c r="P18" s="9"/>
-      <c r="Q18" s="9"/>
-      <c r="R18" s="9"/>
-      <c r="S18" s="9"/>
-      <c r="T18" s="9"/>
-      <c r="U18" s="9"/>
-      <c r="V18" s="9"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="10"/>
+      <c r="N18" s="10"/>
+      <c r="O18" s="10"/>
+      <c r="P18" s="10"/>
+      <c r="Q18" s="10"/>
+      <c r="R18" s="10"/>
+      <c r="S18" s="10"/>
+      <c r="T18" s="10"/>
+      <c r="U18" s="10"/>
+      <c r="V18" s="10"/>
       <c r="W18" s="5"/>
       <c r="X18" s="5"/>
       <c r="Y18" s="5"/>
@@ -1592,19 +1605,19 @@
       <c r="H19" s="2">
         <v>9.2999999999999992E-3</v>
       </c>
-      <c r="J19" s="9"/>
-      <c r="K19" s="9"/>
-      <c r="L19" s="9"/>
-      <c r="M19" s="9"/>
-      <c r="N19" s="9"/>
-      <c r="O19" s="9"/>
-      <c r="P19" s="9"/>
-      <c r="Q19" s="9"/>
-      <c r="R19" s="9"/>
-      <c r="S19" s="9"/>
-      <c r="T19" s="9"/>
-      <c r="U19" s="9"/>
-      <c r="V19" s="9"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="10"/>
+      <c r="M19" s="10"/>
+      <c r="N19" s="10"/>
+      <c r="O19" s="10"/>
+      <c r="P19" s="10"/>
+      <c r="Q19" s="10"/>
+      <c r="R19" s="10"/>
+      <c r="S19" s="10"/>
+      <c r="T19" s="10"/>
+      <c r="U19" s="10"/>
+      <c r="V19" s="10"/>
       <c r="W19" s="5"/>
       <c r="X19" s="5"/>
       <c r="Y19" s="5"/>
@@ -1635,19 +1648,19 @@
       <c r="H20" s="2">
         <v>2.07E-2</v>
       </c>
-      <c r="J20" s="9"/>
-      <c r="K20" s="9"/>
-      <c r="L20" s="9"/>
-      <c r="M20" s="9"/>
-      <c r="N20" s="9"/>
-      <c r="O20" s="9"/>
-      <c r="P20" s="9"/>
-      <c r="Q20" s="9"/>
-      <c r="R20" s="9"/>
-      <c r="S20" s="9"/>
-      <c r="T20" s="9"/>
-      <c r="U20" s="9"/>
-      <c r="V20" s="9"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="10"/>
+      <c r="M20" s="10"/>
+      <c r="N20" s="10"/>
+      <c r="O20" s="10"/>
+      <c r="P20" s="10"/>
+      <c r="Q20" s="10"/>
+      <c r="R20" s="10"/>
+      <c r="S20" s="10"/>
+      <c r="T20" s="10"/>
+      <c r="U20" s="10"/>
+      <c r="V20" s="10"/>
       <c r="W20" s="5"/>
       <c r="X20" s="5"/>
       <c r="Y20" s="5"/>
@@ -1678,19 +1691,19 @@
       <c r="H21" s="2">
         <v>1E-3</v>
       </c>
-      <c r="J21" s="9"/>
-      <c r="K21" s="9"/>
-      <c r="L21" s="9"/>
-      <c r="M21" s="9"/>
-      <c r="N21" s="9"/>
-      <c r="O21" s="9"/>
-      <c r="P21" s="9"/>
-      <c r="Q21" s="9"/>
-      <c r="R21" s="9"/>
-      <c r="S21" s="9"/>
-      <c r="T21" s="9"/>
-      <c r="U21" s="9"/>
-      <c r="V21" s="9"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10"/>
+      <c r="M21" s="10"/>
+      <c r="N21" s="10"/>
+      <c r="O21" s="10"/>
+      <c r="P21" s="10"/>
+      <c r="Q21" s="10"/>
+      <c r="R21" s="10"/>
+      <c r="S21" s="10"/>
+      <c r="T21" s="10"/>
+      <c r="U21" s="10"/>
+      <c r="V21" s="10"/>
       <c r="W21" s="5"/>
       <c r="X21" s="5"/>
       <c r="Y21" s="5"/>
@@ -1721,19 +1734,19 @@
       <c r="H22" s="2">
         <v>8.6999999999999994E-3</v>
       </c>
-      <c r="J22" s="9"/>
-      <c r="K22" s="9"/>
-      <c r="L22" s="9"/>
-      <c r="M22" s="9"/>
-      <c r="N22" s="9"/>
-      <c r="O22" s="9"/>
-      <c r="P22" s="9"/>
-      <c r="Q22" s="9"/>
-      <c r="R22" s="9"/>
-      <c r="S22" s="9"/>
-      <c r="T22" s="9"/>
-      <c r="U22" s="9"/>
-      <c r="V22" s="9"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="10"/>
+      <c r="M22" s="10"/>
+      <c r="N22" s="10"/>
+      <c r="O22" s="10"/>
+      <c r="P22" s="10"/>
+      <c r="Q22" s="10"/>
+      <c r="R22" s="10"/>
+      <c r="S22" s="10"/>
+      <c r="T22" s="10"/>
+      <c r="U22" s="10"/>
+      <c r="V22" s="10"/>
       <c r="W22" s="5"/>
       <c r="X22" s="5"/>
       <c r="Y22" s="5"/>
@@ -1764,19 +1777,19 @@
       <c r="H23" s="2">
         <v>3.5999999999999999E-3</v>
       </c>
-      <c r="J23" s="9"/>
-      <c r="K23" s="9"/>
-      <c r="L23" s="9"/>
-      <c r="M23" s="9"/>
-      <c r="N23" s="9"/>
-      <c r="O23" s="9"/>
-      <c r="P23" s="9"/>
-      <c r="Q23" s="9"/>
-      <c r="R23" s="9"/>
-      <c r="S23" s="9"/>
-      <c r="T23" s="9"/>
-      <c r="U23" s="9"/>
-      <c r="V23" s="9"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="10"/>
+      <c r="M23" s="10"/>
+      <c r="N23" s="10"/>
+      <c r="O23" s="10"/>
+      <c r="P23" s="10"/>
+      <c r="Q23" s="10"/>
+      <c r="R23" s="10"/>
+      <c r="S23" s="10"/>
+      <c r="T23" s="10"/>
+      <c r="U23" s="10"/>
+      <c r="V23" s="10"/>
       <c r="W23" s="5"/>
       <c r="X23" s="5"/>
       <c r="Y23" s="5"/>
@@ -1807,19 +1820,19 @@
       <c r="H24" s="2">
         <v>0</v>
       </c>
-      <c r="J24" s="9"/>
-      <c r="K24" s="9"/>
-      <c r="L24" s="9"/>
-      <c r="M24" s="9"/>
-      <c r="N24" s="9"/>
-      <c r="O24" s="9"/>
-      <c r="P24" s="9"/>
-      <c r="Q24" s="9"/>
-      <c r="R24" s="9"/>
-      <c r="S24" s="9"/>
-      <c r="T24" s="9"/>
-      <c r="U24" s="9"/>
-      <c r="V24" s="9"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="10"/>
+      <c r="L24" s="10"/>
+      <c r="M24" s="10"/>
+      <c r="N24" s="10"/>
+      <c r="O24" s="10"/>
+      <c r="P24" s="10"/>
+      <c r="Q24" s="10"/>
+      <c r="R24" s="10"/>
+      <c r="S24" s="10"/>
+      <c r="T24" s="10"/>
+      <c r="U24" s="10"/>
+      <c r="V24" s="10"/>
       <c r="W24" s="5"/>
       <c r="X24" s="5"/>
       <c r="Y24" s="5"/>
@@ -1850,19 +1863,19 @@
       <c r="H25" s="2">
         <v>1.1000000000000001E-3</v>
       </c>
-      <c r="J25" s="9"/>
-      <c r="K25" s="9"/>
-      <c r="L25" s="9"/>
-      <c r="M25" s="9"/>
-      <c r="N25" s="9"/>
-      <c r="O25" s="9"/>
-      <c r="P25" s="9"/>
-      <c r="Q25" s="9"/>
-      <c r="R25" s="9"/>
-      <c r="S25" s="9"/>
-      <c r="T25" s="9"/>
-      <c r="U25" s="9"/>
-      <c r="V25" s="9"/>
+      <c r="J25" s="10"/>
+      <c r="K25" s="10"/>
+      <c r="L25" s="10"/>
+      <c r="M25" s="10"/>
+      <c r="N25" s="10"/>
+      <c r="O25" s="10"/>
+      <c r="P25" s="10"/>
+      <c r="Q25" s="10"/>
+      <c r="R25" s="10"/>
+      <c r="S25" s="10"/>
+      <c r="T25" s="10"/>
+      <c r="U25" s="10"/>
+      <c r="V25" s="10"/>
       <c r="W25" s="5"/>
       <c r="X25" s="5"/>
       <c r="Y25" s="5"/>
@@ -1893,19 +1906,19 @@
       <c r="H26" s="2">
         <v>1.35E-2</v>
       </c>
-      <c r="J26" s="9"/>
-      <c r="K26" s="9"/>
-      <c r="L26" s="9"/>
-      <c r="M26" s="9"/>
-      <c r="N26" s="9"/>
-      <c r="O26" s="9"/>
-      <c r="P26" s="9"/>
-      <c r="Q26" s="9"/>
-      <c r="R26" s="9"/>
-      <c r="S26" s="9"/>
-      <c r="T26" s="9"/>
-      <c r="U26" s="9"/>
-      <c r="V26" s="9"/>
+      <c r="J26" s="10"/>
+      <c r="K26" s="10"/>
+      <c r="L26" s="10"/>
+      <c r="M26" s="10"/>
+      <c r="N26" s="10"/>
+      <c r="O26" s="10"/>
+      <c r="P26" s="10"/>
+      <c r="Q26" s="10"/>
+      <c r="R26" s="10"/>
+      <c r="S26" s="10"/>
+      <c r="T26" s="10"/>
+      <c r="U26" s="10"/>
+      <c r="V26" s="10"/>
       <c r="W26" s="5"/>
       <c r="X26" s="5"/>
       <c r="Y26" s="5"/>
@@ -1936,19 +1949,19 @@
       <c r="H27" s="2">
         <v>2.1600000000000001E-2</v>
       </c>
-      <c r="J27" s="9"/>
-      <c r="K27" s="9"/>
-      <c r="L27" s="9"/>
-      <c r="M27" s="9"/>
-      <c r="N27" s="9"/>
-      <c r="O27" s="9"/>
-      <c r="P27" s="9"/>
-      <c r="Q27" s="9"/>
-      <c r="R27" s="9"/>
-      <c r="S27" s="9"/>
-      <c r="T27" s="9"/>
-      <c r="U27" s="9"/>
-      <c r="V27" s="9"/>
+      <c r="J27" s="10"/>
+      <c r="K27" s="10"/>
+      <c r="L27" s="10"/>
+      <c r="M27" s="10"/>
+      <c r="N27" s="10"/>
+      <c r="O27" s="10"/>
+      <c r="P27" s="10"/>
+      <c r="Q27" s="10"/>
+      <c r="R27" s="10"/>
+      <c r="S27" s="10"/>
+      <c r="T27" s="10"/>
+      <c r="U27" s="10"/>
+      <c r="V27" s="10"/>
       <c r="W27" s="5"/>
       <c r="X27" s="5"/>
       <c r="Y27" s="5"/>
@@ -1979,19 +1992,19 @@
       <c r="H28" s="2">
         <v>1.9E-3</v>
       </c>
-      <c r="J28" s="9"/>
-      <c r="K28" s="9"/>
-      <c r="L28" s="9"/>
-      <c r="M28" s="9"/>
-      <c r="N28" s="9"/>
-      <c r="O28" s="9"/>
-      <c r="P28" s="9"/>
-      <c r="Q28" s="9"/>
-      <c r="R28" s="9"/>
-      <c r="S28" s="9"/>
-      <c r="T28" s="9"/>
-      <c r="U28" s="9"/>
-      <c r="V28" s="9"/>
+      <c r="J28" s="10"/>
+      <c r="K28" s="10"/>
+      <c r="L28" s="10"/>
+      <c r="M28" s="10"/>
+      <c r="N28" s="10"/>
+      <c r="O28" s="10"/>
+      <c r="P28" s="10"/>
+      <c r="Q28" s="10"/>
+      <c r="R28" s="10"/>
+      <c r="S28" s="10"/>
+      <c r="T28" s="10"/>
+      <c r="U28" s="10"/>
+      <c r="V28" s="10"/>
       <c r="W28" s="5"/>
       <c r="X28" s="5"/>
       <c r="Y28" s="5"/>
@@ -2022,19 +2035,19 @@
       <c r="H29" s="2">
         <v>3.8999999999999998E-3</v>
       </c>
-      <c r="J29" s="9"/>
-      <c r="K29" s="9"/>
-      <c r="L29" s="9"/>
-      <c r="M29" s="9"/>
-      <c r="N29" s="9"/>
-      <c r="O29" s="9"/>
-      <c r="P29" s="9"/>
-      <c r="Q29" s="9"/>
-      <c r="R29" s="9"/>
-      <c r="S29" s="9"/>
-      <c r="T29" s="9"/>
-      <c r="U29" s="9"/>
-      <c r="V29" s="9"/>
+      <c r="J29" s="10"/>
+      <c r="K29" s="10"/>
+      <c r="L29" s="10"/>
+      <c r="M29" s="10"/>
+      <c r="N29" s="10"/>
+      <c r="O29" s="10"/>
+      <c r="P29" s="10"/>
+      <c r="Q29" s="10"/>
+      <c r="R29" s="10"/>
+      <c r="S29" s="10"/>
+      <c r="T29" s="10"/>
+      <c r="U29" s="10"/>
+      <c r="V29" s="10"/>
       <c r="W29" s="5"/>
       <c r="X29" s="5"/>
       <c r="Y29" s="5"/>
@@ -2065,19 +2078,19 @@
       <c r="H30" s="2">
         <v>8.8000000000000005E-3</v>
       </c>
-      <c r="J30" s="9"/>
-      <c r="K30" s="9"/>
-      <c r="L30" s="9"/>
-      <c r="M30" s="9"/>
-      <c r="N30" s="9"/>
-      <c r="O30" s="9"/>
-      <c r="P30" s="9"/>
-      <c r="Q30" s="9"/>
-      <c r="R30" s="9"/>
-      <c r="S30" s="9"/>
-      <c r="T30" s="9"/>
-      <c r="U30" s="9"/>
-      <c r="V30" s="9"/>
+      <c r="J30" s="10"/>
+      <c r="K30" s="10"/>
+      <c r="L30" s="10"/>
+      <c r="M30" s="10"/>
+      <c r="N30" s="10"/>
+      <c r="O30" s="10"/>
+      <c r="P30" s="10"/>
+      <c r="Q30" s="10"/>
+      <c r="R30" s="10"/>
+      <c r="S30" s="10"/>
+      <c r="T30" s="10"/>
+      <c r="U30" s="10"/>
+      <c r="V30" s="10"/>
       <c r="W30" s="5"/>
       <c r="X30" s="5"/>
       <c r="Y30" s="5"/>
@@ -2108,282 +2121,282 @@
       <c r="H31" s="2">
         <v>1.89E-2</v>
       </c>
-      <c r="J31" s="9"/>
-      <c r="K31" s="9"/>
-      <c r="L31" s="9"/>
-      <c r="M31" s="9"/>
-      <c r="N31" s="9"/>
-      <c r="O31" s="9"/>
-      <c r="P31" s="9"/>
-      <c r="Q31" s="9"/>
-      <c r="R31" s="9"/>
-      <c r="S31" s="9"/>
-      <c r="T31" s="9"/>
-      <c r="U31" s="9"/>
-      <c r="V31" s="9"/>
+      <c r="J31" s="10"/>
+      <c r="K31" s="10"/>
+      <c r="L31" s="10"/>
+      <c r="M31" s="10"/>
+      <c r="N31" s="10"/>
+      <c r="O31" s="10"/>
+      <c r="P31" s="10"/>
+      <c r="Q31" s="10"/>
+      <c r="R31" s="10"/>
+      <c r="S31" s="10"/>
+      <c r="T31" s="10"/>
+      <c r="U31" s="10"/>
+      <c r="V31" s="10"/>
       <c r="W31" s="5"/>
       <c r="X31" s="5"/>
       <c r="Y31" s="5"/>
       <c r="Z31" s="5"/>
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="J32" s="9"/>
-      <c r="K32" s="9"/>
-      <c r="L32" s="9"/>
-      <c r="M32" s="9"/>
-      <c r="N32" s="9"/>
-      <c r="O32" s="9"/>
-      <c r="P32" s="9"/>
-      <c r="Q32" s="9"/>
-      <c r="R32" s="9"/>
-      <c r="S32" s="9"/>
-      <c r="T32" s="9"/>
-      <c r="U32" s="9"/>
-      <c r="V32" s="9"/>
+      <c r="J32" s="10"/>
+      <c r="K32" s="10"/>
+      <c r="L32" s="10"/>
+      <c r="M32" s="10"/>
+      <c r="N32" s="10"/>
+      <c r="O32" s="10"/>
+      <c r="P32" s="10"/>
+      <c r="Q32" s="10"/>
+      <c r="R32" s="10"/>
+      <c r="S32" s="10"/>
+      <c r="T32" s="10"/>
+      <c r="U32" s="10"/>
+      <c r="V32" s="10"/>
       <c r="W32" s="5"/>
       <c r="X32" s="5"/>
       <c r="Y32" s="5"/>
       <c r="Z32" s="5"/>
     </row>
     <row r="33" spans="10:22" x14ac:dyDescent="0.25">
-      <c r="J33" s="9"/>
-      <c r="K33" s="9"/>
-      <c r="L33" s="9"/>
-      <c r="M33" s="9"/>
-      <c r="N33" s="9"/>
-      <c r="O33" s="9"/>
-      <c r="P33" s="9"/>
-      <c r="Q33" s="9"/>
-      <c r="R33" s="9"/>
-      <c r="S33" s="9"/>
-      <c r="T33" s="9"/>
-      <c r="U33" s="9"/>
-      <c r="V33" s="9"/>
+      <c r="J33" s="10"/>
+      <c r="K33" s="10"/>
+      <c r="L33" s="10"/>
+      <c r="M33" s="10"/>
+      <c r="N33" s="10"/>
+      <c r="O33" s="10"/>
+      <c r="P33" s="10"/>
+      <c r="Q33" s="10"/>
+      <c r="R33" s="10"/>
+      <c r="S33" s="10"/>
+      <c r="T33" s="10"/>
+      <c r="U33" s="10"/>
+      <c r="V33" s="10"/>
     </row>
     <row r="34" spans="10:22" x14ac:dyDescent="0.25">
-      <c r="J34" s="9"/>
-      <c r="K34" s="9"/>
-      <c r="L34" s="9"/>
-      <c r="M34" s="9"/>
-      <c r="N34" s="9"/>
-      <c r="O34" s="9"/>
-      <c r="P34" s="9"/>
-      <c r="Q34" s="9"/>
-      <c r="R34" s="9"/>
-      <c r="S34" s="9"/>
-      <c r="T34" s="9"/>
-      <c r="U34" s="9"/>
-      <c r="V34" s="9"/>
+      <c r="J34" s="10"/>
+      <c r="K34" s="10"/>
+      <c r="L34" s="10"/>
+      <c r="M34" s="10"/>
+      <c r="N34" s="10"/>
+      <c r="O34" s="10"/>
+      <c r="P34" s="10"/>
+      <c r="Q34" s="10"/>
+      <c r="R34" s="10"/>
+      <c r="S34" s="10"/>
+      <c r="T34" s="10"/>
+      <c r="U34" s="10"/>
+      <c r="V34" s="10"/>
     </row>
     <row r="35" spans="10:22" x14ac:dyDescent="0.25">
-      <c r="J35" s="9"/>
-      <c r="K35" s="9"/>
-      <c r="L35" s="9"/>
-      <c r="M35" s="9"/>
-      <c r="N35" s="9"/>
-      <c r="O35" s="9"/>
-      <c r="P35" s="9"/>
-      <c r="Q35" s="9"/>
-      <c r="R35" s="9"/>
-      <c r="S35" s="9"/>
-      <c r="T35" s="9"/>
-      <c r="U35" s="9"/>
-      <c r="V35" s="9"/>
+      <c r="J35" s="10"/>
+      <c r="K35" s="10"/>
+      <c r="L35" s="10"/>
+      <c r="M35" s="10"/>
+      <c r="N35" s="10"/>
+      <c r="O35" s="10"/>
+      <c r="P35" s="10"/>
+      <c r="Q35" s="10"/>
+      <c r="R35" s="10"/>
+      <c r="S35" s="10"/>
+      <c r="T35" s="10"/>
+      <c r="U35" s="10"/>
+      <c r="V35" s="10"/>
     </row>
     <row r="36" spans="10:22" x14ac:dyDescent="0.25">
-      <c r="J36" s="9"/>
-      <c r="K36" s="9"/>
-      <c r="L36" s="9"/>
-      <c r="M36" s="9"/>
-      <c r="N36" s="9"/>
-      <c r="O36" s="9"/>
-      <c r="P36" s="9"/>
-      <c r="Q36" s="9"/>
-      <c r="R36" s="9"/>
-      <c r="S36" s="9"/>
-      <c r="T36" s="9"/>
-      <c r="U36" s="9"/>
-      <c r="V36" s="9"/>
+      <c r="J36" s="10"/>
+      <c r="K36" s="10"/>
+      <c r="L36" s="10"/>
+      <c r="M36" s="10"/>
+      <c r="N36" s="10"/>
+      <c r="O36" s="10"/>
+      <c r="P36" s="10"/>
+      <c r="Q36" s="10"/>
+      <c r="R36" s="10"/>
+      <c r="S36" s="10"/>
+      <c r="T36" s="10"/>
+      <c r="U36" s="10"/>
+      <c r="V36" s="10"/>
     </row>
     <row r="37" spans="10:22" x14ac:dyDescent="0.25">
-      <c r="J37" s="9"/>
-      <c r="K37" s="9"/>
-      <c r="L37" s="9"/>
-      <c r="M37" s="9"/>
-      <c r="N37" s="9"/>
-      <c r="O37" s="9"/>
-      <c r="P37" s="9"/>
-      <c r="Q37" s="9"/>
-      <c r="R37" s="9"/>
-      <c r="S37" s="9"/>
-      <c r="T37" s="9"/>
-      <c r="U37" s="9"/>
-      <c r="V37" s="9"/>
+      <c r="J37" s="10"/>
+      <c r="K37" s="10"/>
+      <c r="L37" s="10"/>
+      <c r="M37" s="10"/>
+      <c r="N37" s="10"/>
+      <c r="O37" s="10"/>
+      <c r="P37" s="10"/>
+      <c r="Q37" s="10"/>
+      <c r="R37" s="10"/>
+      <c r="S37" s="10"/>
+      <c r="T37" s="10"/>
+      <c r="U37" s="10"/>
+      <c r="V37" s="10"/>
     </row>
     <row r="38" spans="10:22" x14ac:dyDescent="0.25">
-      <c r="J38" s="9"/>
-      <c r="K38" s="9"/>
-      <c r="L38" s="9"/>
-      <c r="M38" s="9"/>
-      <c r="N38" s="9"/>
-      <c r="O38" s="9"/>
-      <c r="P38" s="9"/>
-      <c r="Q38" s="9"/>
-      <c r="R38" s="9"/>
-      <c r="S38" s="9"/>
-      <c r="T38" s="9"/>
-      <c r="U38" s="9"/>
-      <c r="V38" s="9"/>
+      <c r="J38" s="10"/>
+      <c r="K38" s="10"/>
+      <c r="L38" s="10"/>
+      <c r="M38" s="10"/>
+      <c r="N38" s="10"/>
+      <c r="O38" s="10"/>
+      <c r="P38" s="10"/>
+      <c r="Q38" s="10"/>
+      <c r="R38" s="10"/>
+      <c r="S38" s="10"/>
+      <c r="T38" s="10"/>
+      <c r="U38" s="10"/>
+      <c r="V38" s="10"/>
     </row>
     <row r="39" spans="10:22" x14ac:dyDescent="0.25">
-      <c r="J39" s="9"/>
-      <c r="K39" s="9"/>
-      <c r="L39" s="9"/>
-      <c r="M39" s="9"/>
-      <c r="N39" s="9"/>
-      <c r="O39" s="9"/>
-      <c r="P39" s="9"/>
-      <c r="Q39" s="9"/>
-      <c r="R39" s="9"/>
-      <c r="S39" s="9"/>
-      <c r="T39" s="9"/>
-      <c r="U39" s="9"/>
-      <c r="V39" s="9"/>
+      <c r="J39" s="10"/>
+      <c r="K39" s="10"/>
+      <c r="L39" s="10"/>
+      <c r="M39" s="10"/>
+      <c r="N39" s="10"/>
+      <c r="O39" s="10"/>
+      <c r="P39" s="10"/>
+      <c r="Q39" s="10"/>
+      <c r="R39" s="10"/>
+      <c r="S39" s="10"/>
+      <c r="T39" s="10"/>
+      <c r="U39" s="10"/>
+      <c r="V39" s="10"/>
     </row>
     <row r="40" spans="10:22" x14ac:dyDescent="0.25">
-      <c r="J40" s="9"/>
-      <c r="K40" s="9"/>
-      <c r="L40" s="9"/>
-      <c r="M40" s="9"/>
-      <c r="N40" s="9"/>
-      <c r="O40" s="9"/>
-      <c r="P40" s="9"/>
-      <c r="Q40" s="9"/>
-      <c r="R40" s="9"/>
-      <c r="S40" s="9"/>
-      <c r="T40" s="9"/>
-      <c r="U40" s="9"/>
-      <c r="V40" s="9"/>
+      <c r="J40" s="10"/>
+      <c r="K40" s="10"/>
+      <c r="L40" s="10"/>
+      <c r="M40" s="10"/>
+      <c r="N40" s="10"/>
+      <c r="O40" s="10"/>
+      <c r="P40" s="10"/>
+      <c r="Q40" s="10"/>
+      <c r="R40" s="10"/>
+      <c r="S40" s="10"/>
+      <c r="T40" s="10"/>
+      <c r="U40" s="10"/>
+      <c r="V40" s="10"/>
     </row>
     <row r="41" spans="10:22" x14ac:dyDescent="0.25">
-      <c r="J41" s="9"/>
-      <c r="K41" s="9"/>
-      <c r="L41" s="9"/>
-      <c r="M41" s="9"/>
-      <c r="N41" s="9"/>
-      <c r="O41" s="9"/>
-      <c r="P41" s="9"/>
-      <c r="Q41" s="9"/>
-      <c r="R41" s="9"/>
-      <c r="S41" s="9"/>
-      <c r="T41" s="9"/>
-      <c r="U41" s="9"/>
-      <c r="V41" s="9"/>
+      <c r="J41" s="10"/>
+      <c r="K41" s="10"/>
+      <c r="L41" s="10"/>
+      <c r="M41" s="10"/>
+      <c r="N41" s="10"/>
+      <c r="O41" s="10"/>
+      <c r="P41" s="10"/>
+      <c r="Q41" s="10"/>
+      <c r="R41" s="10"/>
+      <c r="S41" s="10"/>
+      <c r="T41" s="10"/>
+      <c r="U41" s="10"/>
+      <c r="V41" s="10"/>
     </row>
     <row r="42" spans="10:22" x14ac:dyDescent="0.25">
-      <c r="J42" s="9"/>
-      <c r="K42" s="9"/>
-      <c r="L42" s="9"/>
-      <c r="M42" s="9"/>
-      <c r="N42" s="9"/>
-      <c r="O42" s="9"/>
-      <c r="P42" s="9"/>
-      <c r="Q42" s="9"/>
-      <c r="R42" s="9"/>
-      <c r="S42" s="9"/>
-      <c r="T42" s="9"/>
-      <c r="U42" s="9"/>
-      <c r="V42" s="9"/>
+      <c r="J42" s="10"/>
+      <c r="K42" s="10"/>
+      <c r="L42" s="10"/>
+      <c r="M42" s="10"/>
+      <c r="N42" s="10"/>
+      <c r="O42" s="10"/>
+      <c r="P42" s="10"/>
+      <c r="Q42" s="10"/>
+      <c r="R42" s="10"/>
+      <c r="S42" s="10"/>
+      <c r="T42" s="10"/>
+      <c r="U42" s="10"/>
+      <c r="V42" s="10"/>
     </row>
     <row r="43" spans="10:22" x14ac:dyDescent="0.25">
-      <c r="J43" s="9"/>
-      <c r="K43" s="9"/>
-      <c r="L43" s="9"/>
-      <c r="M43" s="9"/>
-      <c r="N43" s="9"/>
-      <c r="O43" s="9"/>
-      <c r="P43" s="9"/>
-      <c r="Q43" s="9"/>
-      <c r="R43" s="9"/>
-      <c r="S43" s="9"/>
-      <c r="T43" s="9"/>
-      <c r="U43" s="9"/>
-      <c r="V43" s="9"/>
+      <c r="J43" s="10"/>
+      <c r="K43" s="10"/>
+      <c r="L43" s="10"/>
+      <c r="M43" s="10"/>
+      <c r="N43" s="10"/>
+      <c r="O43" s="10"/>
+      <c r="P43" s="10"/>
+      <c r="Q43" s="10"/>
+      <c r="R43" s="10"/>
+      <c r="S43" s="10"/>
+      <c r="T43" s="10"/>
+      <c r="U43" s="10"/>
+      <c r="V43" s="10"/>
     </row>
     <row r="44" spans="10:22" x14ac:dyDescent="0.25">
-      <c r="J44" s="9"/>
-      <c r="K44" s="9"/>
-      <c r="L44" s="9"/>
-      <c r="M44" s="9"/>
-      <c r="N44" s="9"/>
-      <c r="O44" s="9"/>
-      <c r="P44" s="9"/>
-      <c r="Q44" s="9"/>
-      <c r="R44" s="9"/>
-      <c r="S44" s="9"/>
-      <c r="T44" s="9"/>
-      <c r="U44" s="9"/>
-      <c r="V44" s="9"/>
+      <c r="J44" s="10"/>
+      <c r="K44" s="10"/>
+      <c r="L44" s="10"/>
+      <c r="M44" s="10"/>
+      <c r="N44" s="10"/>
+      <c r="O44" s="10"/>
+      <c r="P44" s="10"/>
+      <c r="Q44" s="10"/>
+      <c r="R44" s="10"/>
+      <c r="S44" s="10"/>
+      <c r="T44" s="10"/>
+      <c r="U44" s="10"/>
+      <c r="V44" s="10"/>
     </row>
     <row r="45" spans="10:22" x14ac:dyDescent="0.25">
-      <c r="J45" s="9"/>
-      <c r="K45" s="9"/>
-      <c r="L45" s="9"/>
-      <c r="M45" s="9"/>
-      <c r="N45" s="9"/>
-      <c r="O45" s="9"/>
-      <c r="P45" s="9"/>
-      <c r="Q45" s="9"/>
-      <c r="R45" s="9"/>
-      <c r="S45" s="9"/>
-      <c r="T45" s="9"/>
-      <c r="U45" s="9"/>
-      <c r="V45" s="9"/>
+      <c r="J45" s="10"/>
+      <c r="K45" s="10"/>
+      <c r="L45" s="10"/>
+      <c r="M45" s="10"/>
+      <c r="N45" s="10"/>
+      <c r="O45" s="10"/>
+      <c r="P45" s="10"/>
+      <c r="Q45" s="10"/>
+      <c r="R45" s="10"/>
+      <c r="S45" s="10"/>
+      <c r="T45" s="10"/>
+      <c r="U45" s="10"/>
+      <c r="V45" s="10"/>
     </row>
     <row r="46" spans="10:22" x14ac:dyDescent="0.25">
-      <c r="J46" s="9"/>
-      <c r="K46" s="9"/>
-      <c r="L46" s="9"/>
-      <c r="M46" s="9"/>
-      <c r="N46" s="9"/>
-      <c r="O46" s="9"/>
-      <c r="P46" s="9"/>
-      <c r="Q46" s="9"/>
-      <c r="R46" s="9"/>
-      <c r="S46" s="9"/>
-      <c r="T46" s="9"/>
-      <c r="U46" s="9"/>
-      <c r="V46" s="9"/>
+      <c r="J46" s="10"/>
+      <c r="K46" s="10"/>
+      <c r="L46" s="10"/>
+      <c r="M46" s="10"/>
+      <c r="N46" s="10"/>
+      <c r="O46" s="10"/>
+      <c r="P46" s="10"/>
+      <c r="Q46" s="10"/>
+      <c r="R46" s="10"/>
+      <c r="S46" s="10"/>
+      <c r="T46" s="10"/>
+      <c r="U46" s="10"/>
+      <c r="V46" s="10"/>
     </row>
     <row r="47" spans="10:22" x14ac:dyDescent="0.25">
-      <c r="J47" s="9"/>
-      <c r="K47" s="9"/>
-      <c r="L47" s="9"/>
-      <c r="M47" s="9"/>
-      <c r="N47" s="9"/>
-      <c r="O47" s="9"/>
-      <c r="P47" s="9"/>
-      <c r="Q47" s="9"/>
-      <c r="R47" s="9"/>
-      <c r="S47" s="9"/>
-      <c r="T47" s="9"/>
-      <c r="U47" s="9"/>
-      <c r="V47" s="9"/>
+      <c r="J47" s="10"/>
+      <c r="K47" s="10"/>
+      <c r="L47" s="10"/>
+      <c r="M47" s="10"/>
+      <c r="N47" s="10"/>
+      <c r="O47" s="10"/>
+      <c r="P47" s="10"/>
+      <c r="Q47" s="10"/>
+      <c r="R47" s="10"/>
+      <c r="S47" s="10"/>
+      <c r="T47" s="10"/>
+      <c r="U47" s="10"/>
+      <c r="V47" s="10"/>
     </row>
     <row r="48" spans="10:22" x14ac:dyDescent="0.25">
-      <c r="J48" s="9"/>
-      <c r="K48" s="9"/>
-      <c r="L48" s="9"/>
-      <c r="M48" s="9"/>
-      <c r="N48" s="9"/>
-      <c r="O48" s="9"/>
-      <c r="P48" s="9"/>
-      <c r="Q48" s="9"/>
-      <c r="R48" s="9"/>
-      <c r="S48" s="9"/>
-      <c r="T48" s="9"/>
-      <c r="U48" s="9"/>
-      <c r="V48" s="9"/>
+      <c r="J48" s="10"/>
+      <c r="K48" s="10"/>
+      <c r="L48" s="10"/>
+      <c r="M48" s="10"/>
+      <c r="N48" s="10"/>
+      <c r="O48" s="10"/>
+      <c r="P48" s="10"/>
+      <c r="Q48" s="10"/>
+      <c r="R48" s="10"/>
+      <c r="S48" s="10"/>
+      <c r="T48" s="10"/>
+      <c r="U48" s="10"/>
+      <c r="V48" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2397,16 +2410,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C6A7977-2381-4943-AA16-A4F852F13E83}">
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.28515625" customWidth="1"/>
     <col min="4" max="4" width="12.85546875" customWidth="1"/>
     <col min="5" max="5" width="38" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="29.42578125" bestFit="1" customWidth="1"/>
@@ -2420,7 +2431,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C1" t="s">
         <v>68</v>
@@ -2429,19 +2440,19 @@
         <v>69</v>
       </c>
       <c r="E1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F1" t="s">
+        <v>95</v>
+      </c>
+      <c r="G1" t="s">
+        <v>96</v>
+      </c>
+      <c r="H1" t="s">
         <v>70</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>71</v>
-      </c>
-      <c r="G1" t="s">
-        <v>72</v>
-      </c>
-      <c r="H1" t="s">
-        <v>73</v>
-      </c>
-      <c r="I1" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -2449,13 +2460,29 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>77</v>
+        <v>74</v>
+      </c>
+      <c r="C2" s="12">
+        <v>1</v>
+      </c>
+      <c r="D2" s="12">
+        <v>10</v>
+      </c>
+      <c r="E2" s="13">
+        <v>0</v>
+      </c>
+      <c r="F2" s="13">
+        <f t="shared" ref="F2:F25" si="0">F3+0.01</f>
+        <v>0.25000000000000006</v>
+      </c>
+      <c r="G2" s="13">
+        <v>0</v>
       </c>
       <c r="H2" s="3">
         <v>0.95099999999999996</v>
       </c>
       <c r="I2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -2463,13 +2490,33 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>76</v>
+        <v>73</v>
+      </c>
+      <c r="C3" s="12">
+        <f>C2+1</f>
+        <v>2</v>
+      </c>
+      <c r="D3" s="12">
+        <f>D2+5</f>
+        <v>15</v>
+      </c>
+      <c r="E3" s="13">
+        <f>E2+0.01</f>
+        <v>0.01</v>
+      </c>
+      <c r="F3" s="13">
+        <f t="shared" si="0"/>
+        <v>0.24000000000000007</v>
+      </c>
+      <c r="G3" s="13">
+        <f>G2+0.01</f>
+        <v>0.01</v>
       </c>
       <c r="H3" s="3">
         <v>0.66100000000000003</v>
       </c>
       <c r="I3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -2477,13 +2524,33 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>76</v>
+        <v>73</v>
+      </c>
+      <c r="C4" s="12">
+        <f t="shared" ref="C4:C27" si="1">C3+1</f>
+        <v>3</v>
+      </c>
+      <c r="D4" s="12">
+        <f t="shared" ref="D4:D27" si="2">D3+5</f>
+        <v>20</v>
+      </c>
+      <c r="E4" s="13">
+        <f t="shared" ref="E4:G27" si="3">E3+0.01</f>
+        <v>0.02</v>
+      </c>
+      <c r="F4" s="13">
+        <f t="shared" si="0"/>
+        <v>0.23000000000000007</v>
+      </c>
+      <c r="G4" s="13">
+        <f t="shared" si="3"/>
+        <v>0.02</v>
       </c>
       <c r="H4" s="3">
         <v>0.55800000000000005</v>
       </c>
       <c r="I4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -2491,13 +2558,33 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>77</v>
+        <v>74</v>
+      </c>
+      <c r="C5" s="12">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="D5" s="12">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="E5" s="13">
+        <f t="shared" si="3"/>
+        <v>0.03</v>
+      </c>
+      <c r="F5" s="13">
+        <f t="shared" si="0"/>
+        <v>0.22000000000000006</v>
+      </c>
+      <c r="G5" s="13">
+        <f t="shared" si="3"/>
+        <v>0.03</v>
       </c>
       <c r="H5" s="3">
         <v>0.90300000000000002</v>
       </c>
       <c r="I5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -2505,13 +2592,33 @@
         <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>78</v>
+        <v>75</v>
+      </c>
+      <c r="C6" s="12">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="D6" s="12">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="E6" s="13">
+        <f t="shared" si="3"/>
+        <v>0.04</v>
+      </c>
+      <c r="F6" s="13">
+        <f t="shared" si="0"/>
+        <v>0.21000000000000005</v>
+      </c>
+      <c r="G6" s="13">
+        <f t="shared" si="3"/>
+        <v>0.04</v>
       </c>
       <c r="H6" s="3">
         <v>0.70499999999999996</v>
       </c>
       <c r="I6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -2519,13 +2626,33 @@
         <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>78</v>
+        <v>75</v>
+      </c>
+      <c r="C7" s="12">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="D7" s="12">
+        <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
+      <c r="E7" s="13">
+        <f t="shared" si="3"/>
+        <v>0.05</v>
+      </c>
+      <c r="F7" s="13">
+        <f t="shared" si="0"/>
+        <v>0.20000000000000004</v>
+      </c>
+      <c r="G7" s="13">
+        <f t="shared" si="3"/>
+        <v>0.05</v>
       </c>
       <c r="H7" s="3">
         <v>0.63300000000000001</v>
       </c>
       <c r="I7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -2533,13 +2660,33 @@
         <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>78</v>
+        <v>75</v>
+      </c>
+      <c r="C8" s="12">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="D8" s="12">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="E8" s="13">
+        <f t="shared" si="3"/>
+        <v>6.0000000000000005E-2</v>
+      </c>
+      <c r="F8" s="13">
+        <f t="shared" si="0"/>
+        <v>0.19000000000000003</v>
+      </c>
+      <c r="G8" s="13">
+        <f t="shared" si="3"/>
+        <v>6.0000000000000005E-2</v>
       </c>
       <c r="H8" s="3">
         <v>0.77400000000000002</v>
       </c>
       <c r="I8" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -2547,13 +2694,33 @@
         <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>78</v>
+        <v>75</v>
+      </c>
+      <c r="C9" s="12">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="D9" s="12">
+        <f t="shared" si="2"/>
+        <v>45</v>
+      </c>
+      <c r="E9" s="13">
+        <f t="shared" si="3"/>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="F9" s="13">
+        <f t="shared" si="0"/>
+        <v>0.18000000000000002</v>
+      </c>
+      <c r="G9" s="13">
+        <f t="shared" si="3"/>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="H9" s="3">
         <v>0.57499999999999996</v>
       </c>
       <c r="I9" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -2561,13 +2728,33 @@
         <v>31</v>
       </c>
       <c r="B10" t="s">
-        <v>78</v>
+        <v>75</v>
+      </c>
+      <c r="C10" s="12">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="D10" s="12">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+      <c r="E10" s="13">
+        <f t="shared" si="3"/>
+        <v>0.08</v>
+      </c>
+      <c r="F10" s="13">
+        <f t="shared" si="0"/>
+        <v>0.17</v>
+      </c>
+      <c r="G10" s="13">
+        <f t="shared" si="3"/>
+        <v>0.08</v>
       </c>
       <c r="H10" s="3">
         <v>0.78200000000000003</v>
       </c>
       <c r="I10" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -2575,13 +2762,33 @@
         <v>33</v>
       </c>
       <c r="B11" t="s">
-        <v>76</v>
+        <v>73</v>
+      </c>
+      <c r="C11" s="12">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="D11" s="12">
+        <f t="shared" si="2"/>
+        <v>55</v>
+      </c>
+      <c r="E11" s="13">
+        <f t="shared" si="3"/>
+        <v>0.09</v>
+      </c>
+      <c r="F11" s="13">
+        <f t="shared" si="0"/>
+        <v>0.16</v>
+      </c>
+      <c r="G11" s="13">
+        <f t="shared" si="3"/>
+        <v>0.09</v>
       </c>
       <c r="H11" s="3">
         <v>0.501</v>
       </c>
       <c r="I11" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -2589,13 +2796,33 @@
         <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>78</v>
+        <v>75</v>
+      </c>
+      <c r="C12" s="12">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="D12" s="12">
+        <f t="shared" si="2"/>
+        <v>60</v>
+      </c>
+      <c r="E12" s="13">
+        <f t="shared" si="3"/>
+        <v>9.9999999999999992E-2</v>
+      </c>
+      <c r="F12" s="13">
+        <f t="shared" si="0"/>
+        <v>0.15</v>
+      </c>
+      <c r="G12" s="13">
+        <f t="shared" si="3"/>
+        <v>9.9999999999999992E-2</v>
       </c>
       <c r="H12" s="3">
         <v>0.747</v>
       </c>
       <c r="I12" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -2603,13 +2830,33 @@
         <v>37</v>
       </c>
       <c r="B13" t="s">
-        <v>76</v>
+        <v>73</v>
+      </c>
+      <c r="C13" s="12">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="D13" s="12">
+        <f t="shared" si="2"/>
+        <v>65</v>
+      </c>
+      <c r="E13" s="13">
+        <f t="shared" si="3"/>
+        <v>0.10999999999999999</v>
+      </c>
+      <c r="F13" s="13">
+        <f t="shared" si="0"/>
+        <v>0.13999999999999999</v>
+      </c>
+      <c r="G13" s="13">
+        <f t="shared" si="3"/>
+        <v>0.10999999999999999</v>
       </c>
       <c r="H13" s="3">
         <v>0.44600000000000001</v>
       </c>
       <c r="I13" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -2617,13 +2864,33 @@
         <v>39</v>
       </c>
       <c r="B14" t="s">
-        <v>78</v>
+        <v>75</v>
+      </c>
+      <c r="C14" s="12">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="D14" s="12">
+        <f t="shared" si="2"/>
+        <v>70</v>
+      </c>
+      <c r="E14" s="13">
+        <f t="shared" si="3"/>
+        <v>0.11999999999999998</v>
+      </c>
+      <c r="F14" s="13">
+        <f t="shared" si="0"/>
+        <v>0.12999999999999998</v>
+      </c>
+      <c r="G14" s="13">
+        <f t="shared" si="3"/>
+        <v>0.11999999999999998</v>
       </c>
       <c r="H14" s="3">
         <v>0.80200000000000005</v>
       </c>
       <c r="I14" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -2631,13 +2898,33 @@
         <v>41</v>
       </c>
       <c r="B15" t="s">
-        <v>78</v>
+        <v>75</v>
+      </c>
+      <c r="C15" s="12">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="D15" s="12">
+        <f t="shared" si="2"/>
+        <v>75</v>
+      </c>
+      <c r="E15" s="13">
+        <f t="shared" si="3"/>
+        <v>0.12999999999999998</v>
+      </c>
+      <c r="F15" s="13">
+        <f t="shared" si="0"/>
+        <v>0.11999999999999998</v>
+      </c>
+      <c r="G15" s="13">
+        <f t="shared" si="3"/>
+        <v>0.12999999999999998</v>
       </c>
       <c r="H15" s="3">
         <v>0.80300000000000005</v>
       </c>
       <c r="I15" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -2645,13 +2932,33 @@
         <v>43</v>
       </c>
       <c r="B16" t="s">
-        <v>78</v>
+        <v>75</v>
+      </c>
+      <c r="C16" s="12">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="D16" s="12">
+        <f t="shared" si="2"/>
+        <v>80</v>
+      </c>
+      <c r="E16" s="13">
+        <f t="shared" si="3"/>
+        <v>0.13999999999999999</v>
+      </c>
+      <c r="F16" s="13">
+        <f t="shared" si="0"/>
+        <v>0.10999999999999999</v>
+      </c>
+      <c r="G16" s="13">
+        <f t="shared" si="3"/>
+        <v>0.13999999999999999</v>
       </c>
       <c r="H16" s="3">
         <v>0.81599999999999995</v>
       </c>
       <c r="I16" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -2659,13 +2966,33 @@
         <v>45</v>
       </c>
       <c r="B17" t="s">
-        <v>78</v>
+        <v>75</v>
+      </c>
+      <c r="C17" s="12">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="D17" s="12">
+        <f t="shared" si="2"/>
+        <v>85</v>
+      </c>
+      <c r="E17" s="13">
+        <f t="shared" si="3"/>
+        <v>0.15</v>
+      </c>
+      <c r="F17" s="13">
+        <f t="shared" si="0"/>
+        <v>9.9999999999999992E-2</v>
+      </c>
+      <c r="G17" s="13">
+        <f t="shared" si="3"/>
+        <v>0.15</v>
       </c>
       <c r="H17" s="3">
         <v>0.54400000000000004</v>
       </c>
       <c r="I17" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -2673,13 +3000,33 @@
         <v>49</v>
       </c>
       <c r="B18" t="s">
-        <v>76</v>
+        <v>73</v>
+      </c>
+      <c r="C18" s="12">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="D18" s="12">
+        <f t="shared" si="2"/>
+        <v>90</v>
+      </c>
+      <c r="E18" s="13">
+        <f t="shared" si="3"/>
+        <v>0.16</v>
+      </c>
+      <c r="F18" s="13">
+        <f t="shared" si="0"/>
+        <v>0.09</v>
+      </c>
+      <c r="G18" s="13">
+        <f t="shared" si="3"/>
+        <v>0.16</v>
       </c>
       <c r="H18" s="3">
         <v>0.50800000000000001</v>
       </c>
       <c r="I18" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -2687,13 +3034,33 @@
         <v>51</v>
       </c>
       <c r="B19" t="s">
-        <v>76</v>
+        <v>73</v>
+      </c>
+      <c r="C19" s="12">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="D19" s="12">
+        <f t="shared" si="2"/>
+        <v>95</v>
+      </c>
+      <c r="E19" s="13">
+        <f t="shared" si="3"/>
+        <v>0.17</v>
+      </c>
+      <c r="F19" s="13">
+        <f t="shared" si="0"/>
+        <v>0.08</v>
+      </c>
+      <c r="G19" s="13">
+        <f t="shared" si="3"/>
+        <v>0.17</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="I19" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -2701,13 +3068,33 @@
         <v>53</v>
       </c>
       <c r="B20" t="s">
-        <v>78</v>
+        <v>75</v>
+      </c>
+      <c r="C20" s="12">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="D20" s="12">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="E20" s="13">
+        <f t="shared" si="3"/>
+        <v>0.18000000000000002</v>
+      </c>
+      <c r="F20" s="13">
+        <f t="shared" si="0"/>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G20" s="13">
+        <f t="shared" si="3"/>
+        <v>0.18000000000000002</v>
       </c>
       <c r="H20" s="3">
         <v>0.78500000000000003</v>
       </c>
       <c r="I20" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -2715,13 +3102,33 @@
         <v>55</v>
       </c>
       <c r="B21" t="s">
-        <v>78</v>
+        <v>75</v>
+      </c>
+      <c r="C21" s="12">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="D21" s="12">
+        <f t="shared" si="2"/>
+        <v>105</v>
+      </c>
+      <c r="E21" s="13">
+        <f t="shared" si="3"/>
+        <v>0.19000000000000003</v>
+      </c>
+      <c r="F21" s="13">
+        <f t="shared" si="0"/>
+        <v>6.0000000000000005E-2</v>
+      </c>
+      <c r="G21" s="13">
+        <f t="shared" si="3"/>
+        <v>0.19000000000000003</v>
       </c>
       <c r="H21" s="3">
         <v>0.8</v>
       </c>
       <c r="I21" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -2729,13 +3136,33 @@
         <v>57</v>
       </c>
       <c r="B22" t="s">
-        <v>76</v>
+        <v>73</v>
+      </c>
+      <c r="C22" s="12">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="D22" s="12">
+        <f t="shared" si="2"/>
+        <v>110</v>
+      </c>
+      <c r="E22" s="13">
+        <f t="shared" si="3"/>
+        <v>0.20000000000000004</v>
+      </c>
+      <c r="F22" s="13">
+        <f t="shared" si="0"/>
+        <v>0.05</v>
+      </c>
+      <c r="G22" s="13">
+        <f t="shared" si="3"/>
+        <v>0.20000000000000004</v>
       </c>
       <c r="H22" s="3">
         <v>0.54900000000000004</v>
       </c>
       <c r="I22" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -2743,13 +3170,33 @@
         <v>59</v>
       </c>
       <c r="B23" t="s">
-        <v>76</v>
+        <v>73</v>
+      </c>
+      <c r="C23" s="12">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="D23" s="12">
+        <f t="shared" si="2"/>
+        <v>115</v>
+      </c>
+      <c r="E23" s="13">
+        <f t="shared" si="3"/>
+        <v>0.21000000000000005</v>
+      </c>
+      <c r="F23" s="13">
+        <f t="shared" si="0"/>
+        <v>0.04</v>
+      </c>
+      <c r="G23" s="13">
+        <f t="shared" si="3"/>
+        <v>0.21000000000000005</v>
       </c>
       <c r="H23" s="3">
         <v>0.45500000000000002</v>
       </c>
       <c r="I23" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -2757,13 +3204,33 @@
         <v>61</v>
       </c>
       <c r="B24" t="s">
-        <v>78</v>
+        <v>75</v>
+      </c>
+      <c r="C24" s="12">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="D24" s="12">
+        <f t="shared" si="2"/>
+        <v>120</v>
+      </c>
+      <c r="E24" s="13">
+        <f t="shared" si="3"/>
+        <v>0.22000000000000006</v>
+      </c>
+      <c r="F24" s="13">
+        <f t="shared" si="0"/>
+        <v>0.03</v>
+      </c>
+      <c r="G24" s="13">
+        <f t="shared" si="3"/>
+        <v>0.22000000000000006</v>
       </c>
       <c r="H24" s="3">
         <v>0.71299999999999997</v>
       </c>
       <c r="I24" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -2771,13 +3238,33 @@
         <v>15</v>
       </c>
       <c r="B25" t="s">
-        <v>77</v>
+        <v>74</v>
+      </c>
+      <c r="C25" s="12">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="D25" s="12">
+        <f t="shared" si="2"/>
+        <v>125</v>
+      </c>
+      <c r="E25" s="13">
+        <f t="shared" si="3"/>
+        <v>0.23000000000000007</v>
+      </c>
+      <c r="F25" s="13">
+        <f t="shared" si="0"/>
+        <v>0.02</v>
+      </c>
+      <c r="G25" s="13">
+        <f t="shared" si="3"/>
+        <v>0.23000000000000007</v>
       </c>
       <c r="H25" s="3">
         <v>0.92900000000000005</v>
       </c>
       <c r="I25" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -2785,48 +3272,77 @@
         <v>11</v>
       </c>
       <c r="B26" t="s">
-        <v>77</v>
+        <v>74</v>
+      </c>
+      <c r="C26" s="12">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="D26" s="12">
+        <f t="shared" si="2"/>
+        <v>130</v>
+      </c>
+      <c r="E26" s="13">
+        <f t="shared" si="3"/>
+        <v>0.24000000000000007</v>
+      </c>
+      <c r="F26" s="13">
+        <f>F27+0.01</f>
+        <v>0.01</v>
+      </c>
+      <c r="G26" s="13">
+        <f t="shared" si="3"/>
+        <v>0.24000000000000007</v>
       </c>
       <c r="H26" s="3">
         <v>0.89610000000000001</v>
       </c>
       <c r="I26" t="s">
-        <v>83</v>
-      </c>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B28" t="s">
-        <v>92</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>93</v>
+        <v>89</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>82</v>
-      </c>
-      <c r="C29" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>94</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>95</v>
+        <v>91</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>91</v>
-      </c>
-      <c r="C31" s="10" t="s">
-        <v>96</v>
+        <v>88</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" s="12" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -2837,5 +3353,8 @@
     <hyperlink ref="C31" r:id="rId4" xr:uid="{4A9C1AAE-88CB-4671-8792-DBBE075D16B9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="F3:F26" formula="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>